<commit_message>
dis assembler now supports all basic ch8 instructions with a few issues
</commit_message>
<xml_diff>
--- a/docs/chip8opcodeList.xlsx
+++ b/docs/chip8opcodeList.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="99">
   <si>
     <t xml:space="preserve">Opcode</t>
   </si>
@@ -31,6 +31,9 @@
     <t xml:space="preserve">In Assembler</t>
   </si>
   <si>
+    <t xml:space="preserve">In Disassembler</t>
+  </si>
+  <si>
     <t xml:space="preserve">In emulator</t>
   </si>
   <si>
@@ -43,6 +46,9 @@
     <t xml:space="preserve"> CLS</t>
   </si>
   <si>
+    <t xml:space="preserve">X</t>
+  </si>
+  <si>
     <t xml:space="preserve">            0x00EE </t>
   </si>
   <si>
@@ -55,6 +61,9 @@
     <t xml:space="preserve"> SYS addr</t>
   </si>
   <si>
+    <t xml:space="preserve">Used by older computers and should be ignored</t>
+  </si>
+  <si>
     <t xml:space="preserve">            1nnn </t>
   </si>
   <si>
@@ -251,6 +260,9 @@
   </si>
   <si>
     <t xml:space="preserve"> SCD nibble</t>
+  </si>
+  <si>
+    <t xml:space="preserve">super chip8</t>
   </si>
   <si>
     <t xml:space="preserve">            00FB </t>
@@ -320,6 +332,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -475,17 +488,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.72"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.28"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -504,365 +519,503 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>24</v>
+        <v>27</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>30</v>
+        <v>33</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>32</v>
+        <v>35</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>78</v>
+        <v>82</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B39" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="F39" s="0" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>82</v>
+        <v>86</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>84</v>
+        <v>88</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>86</v>
+        <v>90</v>
+      </c>
+      <c r="F42" s="0" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>88</v>
+        <v>92</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>90</v>
+        <v>94</v>
+      </c>
+      <c r="F44" s="0" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>92</v>
+        <v>96</v>
+      </c>
+      <c r="F45" s="0" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>94</v>
+        <v>98</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>